<commit_message>
- sửa update cell exels có thể map được cell kéo dài
</commit_message>
<xml_diff>
--- a/src/main/webapp/resources/excel/Template_CAPNHAT_CELL_2G.xlsx
+++ b/src/main/webapp/resources/excel/Template_CAPNHAT_CELL_2G.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VNPT\RIMS\trunk\code\RIMS\src\main\webapp\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trunglk\Project\RIMS_GIT\RIMS_GITLAB_HUU\src\main\webapp\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FDEB45AD-E47F-4A09-B43A-6BC51CFB2AAD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="331"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="331" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cập nhật CELL 2G" sheetId="10" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="11" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cập nhật CELL 2G'!$D$2:$U$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cập nhật CELL 2G'!$F$2:$W$3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>Thông tin khai sinh</t>
   </si>
@@ -209,17 +210,29 @@
   </si>
   <si>
     <t>Mã CELL2G</t>
+  </si>
+  <si>
+    <t>Cell kéo dài</t>
+  </si>
+  <si>
+    <t>Cell Thường</t>
+  </si>
+  <si>
+    <t>Mã CSHT</t>
+  </si>
+  <si>
+    <t>CSHT_NTN_00001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -256,7 +269,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -264,7 +277,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -295,7 +308,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -315,19 +328,6 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -368,26 +368,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -402,7 +382,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -411,10 +391,7 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -431,40 +408,46 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 107" xfId="3"/>
-    <cellStyle name="Normal 2 11" xfId="4"/>
-    <cellStyle name="Normal 2 113" xfId="5"/>
-    <cellStyle name="Normal 2 119" xfId="6"/>
-    <cellStyle name="Normal 2 2 10 2" xfId="7"/>
-    <cellStyle name="Normal 2 51" xfId="8"/>
-    <cellStyle name="Normal 2 61" xfId="9"/>
-    <cellStyle name="Normal 2 70" xfId="10"/>
+    <cellStyle name="Normal 10" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 107" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2 11" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2 113" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 119" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 10 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2 51" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 2 61" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 2 70" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -799,316 +782,423 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AL4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="26.375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.375" customWidth="1"/>
-    <col min="6" max="6" width="19.375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="18.375" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.375" customWidth="1"/>
-    <col min="14" max="14" width="18.375" style="6" customWidth="1"/>
-    <col min="15" max="15" width="18.375" customWidth="1"/>
-    <col min="16" max="21" width="18.375" style="6" customWidth="1"/>
-    <col min="22" max="22" width="18" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="26.375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.25" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="18.42578125" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
+    <col min="14" max="14" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" style="5" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
+    <col min="18" max="23" width="18.42578125" style="5" customWidth="1"/>
+    <col min="24" max="24" width="18" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="24.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:38" ht="24.75" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="17"/>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="12" t="s">
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="14"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="13"/>
     </row>
-    <row r="2" spans="1:37" ht="22.5" customHeight="1">
-      <c r="A2" s="15"/>
+    <row r="2" spans="1:38" ht="22.5" customHeight="1">
+      <c r="A2" s="14"/>
       <c r="B2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AJ2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AK2" s="3" t="s">
+      <c r="AL2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
-      <c r="A3" s="8"/>
+    <row r="3" spans="1:38">
+      <c r="A3" s="7"/>
       <c r="B3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="1">
+      <c r="J3" s="1">
         <v>5</v>
       </c>
-      <c r="I3" s="1">
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="P3" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="1">
+      <c r="Q3" s="1">
         <v>1</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="R3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="S3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="T3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="U3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="V3" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="W3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="7">
+      <c r="X3" s="6">
         <v>1</v>
       </c>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7" t="s">
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38">
+      <c r="A4" s="7"/>
+      <c r="B4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="X4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6" t="s">
         <v>55</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="V1:AK1"/>
+  <mergeCells count="7">
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="P1:U1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="I1:M1"/>
     <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="X1:AL1"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{E5174E4B-2840-4EBB-82AA-0B204988B5D2}">
+      <formula1>"Cell Thường, Cell kéo dài"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>